<commit_message>
Added cert nacimiento and Budget Database update
</commit_message>
<xml_diff>
--- a/Budget Database.xlsx
+++ b/Budget Database.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agalindoes002\Desktop\AGalindoEscobedo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDC17EF5-835E-4E9F-8033-C06F91A7A263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC89C82-DDD5-4AA0-BA14-121DE692B3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32685" yWindow="2520" windowWidth="21600" windowHeight="12645" xr2:uid="{F3AB8A3D-EA62-4C75-965C-AA387736434D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{F3AB8A3D-EA62-4C75-965C-AA387736434D}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Transaction</t>
   </si>
@@ -75,16 +76,133 @@
   </si>
   <si>
     <t>Clothes</t>
+  </si>
+  <si>
+    <t>John Harris</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billa </t>
+  </si>
+  <si>
+    <t>Viaje Bratislava</t>
+  </si>
+  <si>
+    <t>Entretenimiento</t>
+  </si>
+  <si>
+    <t>Der Mann</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Wohnen</t>
+  </si>
+  <si>
+    <t>ORF Beitrag</t>
+  </si>
+  <si>
+    <t>ATM</t>
+  </si>
+  <si>
+    <t>Miso Supermarkt</t>
+  </si>
+  <si>
+    <t>Cafe Caspar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jewelry </t>
+  </si>
+  <si>
+    <t>Pho</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>Gotas Ojos</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Bildung</t>
+  </si>
+  <si>
+    <t>24/7 Shop</t>
+  </si>
+  <si>
+    <t>Prime Video</t>
+  </si>
+  <si>
+    <t>Hielo</t>
+  </si>
+  <si>
+    <t>dpb.sk</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Graz</t>
+  </si>
+  <si>
+    <t>Cafe</t>
+  </si>
+  <si>
+    <t>Liebling</t>
+  </si>
+  <si>
+    <t>Chez Bernard</t>
+  </si>
+  <si>
+    <t>Dampha</t>
+  </si>
+  <si>
+    <t>Comida Mashi</t>
+  </si>
+  <si>
+    <t>Uno Kitchen</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Comida /entretenimiento /salud etc</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>apartamento + internet</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>PwC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +210,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,15 +239,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,116 +581,706 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F122AF-52CD-4ABC-A912-D47727141FD0}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="1" max="1" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45393</v>
+      </c>
+      <c r="D2" s="7">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>45398</v>
+      </c>
+      <c r="D3" s="7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45407</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
+        <v>45407</v>
+      </c>
+      <c r="D5" s="7">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45408</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>45408</v>
+      </c>
+      <c r="D7" s="7">
+        <v>8.1199999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6">
+        <v>45413</v>
+      </c>
+      <c r="D8" s="7">
+        <v>70.849999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6">
+        <v>45413</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D11" s="7">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SUM(D8:D30)</f>
+        <v>469.64000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D12" s="7">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D13" s="7">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1">
+        <f>SUM(D31:D43)</f>
+        <v>200.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D15" s="7">
+        <v>6.99</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="1">
+        <f>(H11+H13)*2</f>
+        <v>1340.64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="6">
+        <v>45414</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6">
+        <v>45415</v>
+      </c>
+      <c r="D17" s="7">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>45415</v>
+      </c>
+      <c r="D18" s="7">
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6">
+        <v>45415</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="6">
+        <v>45415</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6">
+        <v>45416</v>
+      </c>
+      <c r="D21" s="7">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6">
+        <v>45416</v>
+      </c>
+      <c r="D22" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="6">
+        <v>45416</v>
+      </c>
+      <c r="D23" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6">
+        <v>45416</v>
+      </c>
+      <c r="D24" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="6">
+        <v>45416</v>
+      </c>
+      <c r="D25" s="7">
+        <v>10.49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="6">
+        <v>45418</v>
+      </c>
+      <c r="D26" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="6">
+        <v>45418</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="6">
+        <v>45418</v>
+      </c>
+      <c r="D28" s="7">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="6">
+        <v>45418</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="6">
+        <v>45418</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="6">
+        <v>45423</v>
+      </c>
+      <c r="D31" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="6">
+        <v>45423</v>
+      </c>
+      <c r="D32" s="7">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="6">
+        <v>45422</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="6">
+        <v>45422</v>
+      </c>
+      <c r="D34" s="7">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="6">
+        <v>45422</v>
+      </c>
+      <c r="D35" s="7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="6">
+        <v>45422</v>
+      </c>
+      <c r="D36" s="7">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="6">
+        <v>45421</v>
+      </c>
+      <c r="D37" s="7">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="6">
+        <v>45420</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="6">
+        <v>45420</v>
+      </c>
+      <c r="D39" s="7">
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="6">
+        <v>45420</v>
+      </c>
+      <c r="D40" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="6">
+        <v>45425</v>
+      </c>
+      <c r="D41" s="7">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="6">
+        <v>45425</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="6">
+        <v>45425</v>
+      </c>
+      <c r="D43" s="7">
+        <v>4.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D30">
+    <sortCondition ref="C1:C30"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3978A1-FA3B-4904-B4D7-61C52F949AF0}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45408</v>
-      </c>
-      <c r="D2" s="3">
-        <v>6.96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2">
+        <v>2789.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45398</v>
-      </c>
-      <c r="D3" s="3">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>1340.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45393</v>
-      </c>
-      <c r="D4" s="3">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E4">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45408</v>
-      </c>
-      <c r="D5" s="3">
-        <v>8.1199999999999992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45407</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45407</v>
-      </c>
-      <c r="D7" s="3">
-        <v>19.989999999999998</v>
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <f>E3+E4</f>
+        <v>1775.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>